<commit_message>
ajuste de campos 2
</commit_message>
<xml_diff>
--- a/Teste Faturamento.xlsx
+++ b/Teste Faturamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucca.peixoto\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04026089-D0E2-4F1C-B9AF-F6504409C43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E714A4-E236-49DF-9FA8-E611F05E38A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E49487A5-60F5-451E-8CC0-EC090C6FFE99}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>Devolução (Promotores)</t>
   </si>
   <si>
-    <t>Tendência</t>
-  </si>
-  <si>
     <t>Tendência (%)</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>Real_Gerente</t>
+  </si>
+  <si>
+    <t>Tendência_Gerente</t>
   </si>
 </sst>
 </file>
@@ -565,9 +565,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,6 +597,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -963,14 +963,14 @@
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -982,7 +982,7 @@
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="53" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -1000,14 +1000,14 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>2</v>
@@ -1028,13 +1028,13 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="N1" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>16</v>
@@ -1042,20 +1042,20 @@
       <c r="P1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="50" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="11" t="s">
         <v>20</v>
       </c>
       <c r="T1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="V1" s="19" t="s">
         <v>22</v>
@@ -1064,36 +1064,36 @@
         <v>23</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="55" t="s">
+      <c r="Z1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="56" t="s">
+      <c r="AA1" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="55" t="s">
+      <c r="AB1" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="AC1" s="19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="49">
+      <c r="B2" s="48">
         <v>11100000</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="44">
         <f>SUM(K2:K6)</f>
         <v>10071948.34</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="58">
         <f>(C2/G2) * F2</f>
         <v>12589935.425000001</v>
       </c>
@@ -1111,17 +1111,17 @@
         <v>9</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="47">
+        <v>60</v>
+      </c>
+      <c r="J2" s="46">
         <f>SUM(Q10,Q9,Q2,Q17)</f>
         <v>1062606.44</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="47">
         <f>SUM(R2,R9:R10,R20,R17)</f>
         <v>1870000</v>
       </c>
-      <c r="L2" s="48">
+      <c r="L2" s="47">
         <f>(K2/G2) * F2</f>
         <v>2337500</v>
       </c>
@@ -1133,15 +1133,15 @@
         <v>9</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="52">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="51">
         <v>509039.59</v>
       </c>
-      <c r="R2" s="48">
+      <c r="R2" s="47">
         <v>400000</v>
       </c>
       <c r="S2" s="14">
@@ -1162,18 +1162,18 @@
         <v>10</v>
       </c>
       <c r="X2" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="57">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="56">
         <v>278034.96999999997</v>
       </c>
-      <c r="Z2" s="58">
+      <c r="Z2" s="57">
         <v>226461.61</v>
       </c>
-      <c r="AA2" s="58">
+      <c r="AA2" s="57">
         <v>0</v>
       </c>
-      <c r="AB2" s="58">
+      <c r="AB2" s="57">
         <f>(Z2/G2) * F2</f>
         <v>283077.01250000001</v>
       </c>
@@ -1191,15 +1191,15 @@
       <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="49">
+      <c r="J3" s="48">
         <f>SUM(Q5,Q11,Q12,Q14,Q18)</f>
         <v>1291110.55</v>
       </c>
-      <c r="K3" s="48">
+      <c r="K3" s="47">
         <f>SUM(R5,R11,R12,R14,R18,R19)</f>
         <v>2470000</v>
       </c>
-      <c r="L3" s="48">
+      <c r="L3" s="47">
         <f>(K3/G2) * F2</f>
         <v>3087500</v>
       </c>
@@ -1214,12 +1214,12 @@
         <v>14</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="52">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="51">
         <v>112244.82</v>
       </c>
-      <c r="R3" s="48">
+      <c r="R3" s="47">
         <v>420000</v>
       </c>
       <c r="S3" s="14">
@@ -1240,18 +1240,18 @@
         <v>10</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y3" s="57">
+        <v>51</v>
+      </c>
+      <c r="Y3" s="56">
         <v>359768.99</v>
       </c>
-      <c r="Z3" s="58">
+      <c r="Z3" s="57">
         <v>233197.73</v>
       </c>
-      <c r="AA3" s="58">
+      <c r="AA3" s="57">
         <v>0</v>
       </c>
-      <c r="AB3" s="58">
+      <c r="AB3" s="57">
         <f>(Z3/G2) * F2</f>
         <v>291497.16250000003</v>
       </c>
@@ -1273,11 +1273,11 @@
         <f>SUM(Q7,Q15:Q16,Q4,Q6,Q8)</f>
         <v>1675335.7400000002</v>
       </c>
-      <c r="K4" s="48">
+      <c r="K4" s="47">
         <f>SUM(R6:R8,R15:R16,R4,R21)</f>
         <v>2840000</v>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="47">
         <f>(K4/G2) * F2</f>
         <v>3550000</v>
       </c>
@@ -1292,12 +1292,12 @@
         <v>12</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q4" s="52">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="51">
         <v>77301.78</v>
       </c>
-      <c r="R4" s="48">
+      <c r="R4" s="47">
         <v>430000</v>
       </c>
       <c r="S4" s="14">
@@ -1318,18 +1318,18 @@
         <v>10</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y4" s="57">
+        <v>32</v>
+      </c>
+      <c r="Y4" s="56">
         <v>309362.19</v>
       </c>
-      <c r="Z4" s="58">
+      <c r="Z4" s="57">
         <v>344774.33</v>
       </c>
-      <c r="AA4" s="58">
+      <c r="AA4" s="57">
         <v>0</v>
       </c>
-      <c r="AB4" s="58">
+      <c r="AB4" s="57">
         <f>(Z4/G2) * F2</f>
         <v>430967.91250000003</v>
       </c>
@@ -1347,15 +1347,15 @@
       <c r="I5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="48">
         <f>SUM(Q3:Q3,Q13,Y10)</f>
         <v>205818.47</v>
       </c>
-      <c r="K5" s="48">
+      <c r="K5" s="47">
         <f>SUM(R3:R3,R13,Z10,R23)</f>
         <v>967093.47</v>
       </c>
-      <c r="L5" s="48">
+      <c r="L5" s="47">
         <f>(K5/G2) * F2</f>
         <v>1208866.8374999999</v>
       </c>
@@ -1370,12 +1370,12 @@
         <v>11</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" s="52">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="51">
         <v>233605.43</v>
       </c>
-      <c r="R5" s="48">
+      <c r="R5" s="47">
         <v>440000</v>
       </c>
       <c r="S5" s="14">
@@ -1396,18 +1396,18 @@
         <v>10</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y5" s="57">
+        <v>52</v>
+      </c>
+      <c r="Y5" s="56">
         <v>106150.22</v>
       </c>
-      <c r="Z5" s="58">
+      <c r="Z5" s="57">
         <v>123622.36</v>
       </c>
-      <c r="AA5" s="58">
+      <c r="AA5" s="57">
         <v>0</v>
       </c>
-      <c r="AB5" s="58">
+      <c r="AB5" s="57">
         <f>(Z5/G2) * F2</f>
         <v>154527.95000000001</v>
       </c>
@@ -1425,15 +1425,15 @@
       <c r="I6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="49">
+      <c r="J6" s="48">
         <f>SUM(Y2:Y9)</f>
         <v>2015141.99</v>
       </c>
-      <c r="K6" s="48">
+      <c r="K6" s="47">
         <f>SUM(Z2:Z9)</f>
         <v>1924854.87</v>
       </c>
-      <c r="L6" s="48">
+      <c r="L6" s="47">
         <f>(K6/G2) * F2</f>
         <v>2406068.5875000004</v>
       </c>
@@ -1448,12 +1448,12 @@
         <v>12</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" s="52">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="51">
         <v>240901.6</v>
       </c>
-      <c r="R6" s="48">
+      <c r="R6" s="47">
         <v>450000</v>
       </c>
       <c r="S6" s="14">
@@ -1474,18 +1474,18 @@
         <v>10</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="57">
+        <v>33</v>
+      </c>
+      <c r="Y6" s="56">
         <v>253882.6</v>
       </c>
-      <c r="Z6" s="58">
+      <c r="Z6" s="57">
         <v>264703.65000000002</v>
       </c>
-      <c r="AA6" s="58">
+      <c r="AA6" s="57">
         <v>0</v>
       </c>
-      <c r="AB6" s="58">
+      <c r="AB6" s="57">
         <f>(Z6/G2) * F2</f>
         <v>330879.5625</v>
       </c>
@@ -1504,12 +1504,12 @@
         <v>12</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="52">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="51">
         <v>375146.39</v>
       </c>
-      <c r="R7" s="48">
+      <c r="R7" s="47">
         <v>460000</v>
       </c>
       <c r="S7" s="14">
@@ -1530,18 +1530,18 @@
         <v>10</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y7" s="57">
+        <v>53</v>
+      </c>
+      <c r="Y7" s="56">
         <v>235058.47</v>
       </c>
-      <c r="Z7" s="58">
+      <c r="Z7" s="57">
         <v>236058.57</v>
       </c>
-      <c r="AA7" s="58">
+      <c r="AA7" s="57">
         <v>0</v>
       </c>
-      <c r="AB7" s="58">
+      <c r="AB7" s="57">
         <f>(Z7/G2) * F2</f>
         <v>295073.21250000002</v>
       </c>
@@ -1560,12 +1560,12 @@
         <v>12</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q8" s="52">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="51">
         <v>450561.05</v>
       </c>
-      <c r="R8" s="48">
+      <c r="R8" s="47">
         <v>460000</v>
       </c>
       <c r="S8" s="14">
@@ -1586,18 +1586,18 @@
         <v>10</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y8" s="57">
+        <v>54</v>
+      </c>
+      <c r="Y8" s="56">
         <v>263862.83</v>
       </c>
-      <c r="Z8" s="58">
+      <c r="Z8" s="57">
         <v>245292.27</v>
       </c>
-      <c r="AA8" s="58">
+      <c r="AA8" s="57">
         <v>0</v>
       </c>
-      <c r="AB8" s="58">
+      <c r="AB8" s="57">
         <f>(Z8/G2) * F2</f>
         <v>306615.33749999997</v>
       </c>
@@ -1613,15 +1613,15 @@
         <v>9</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q9" s="52">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="51">
         <v>149058.19</v>
       </c>
-      <c r="R9" s="48">
+      <c r="R9" s="47">
         <v>470000</v>
       </c>
       <c r="S9" s="14">
@@ -1642,18 +1642,18 @@
         <v>10</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y9" s="57">
+        <v>55</v>
+      </c>
+      <c r="Y9" s="56">
         <v>209021.72</v>
       </c>
-      <c r="Z9" s="58">
+      <c r="Z9" s="57">
         <v>250744.35</v>
       </c>
-      <c r="AA9" s="58">
+      <c r="AA9" s="57">
         <v>0</v>
       </c>
-      <c r="AB9" s="58">
+      <c r="AB9" s="57">
         <f>(Z9/G2) * F2</f>
         <v>313430.4375</v>
       </c>
@@ -1669,15 +1669,15 @@
         <v>9</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q10" s="52">
+        <v>62</v>
+      </c>
+      <c r="Q10" s="51">
         <v>230480.73</v>
       </c>
-      <c r="R10" s="48">
+      <c r="R10" s="47">
         <v>480000</v>
       </c>
       <c r="S10" s="14">
@@ -1698,15 +1698,15 @@
         <v>14</v>
       </c>
       <c r="X10" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Y10" s="40">
         <v>51752.1</v>
       </c>
-      <c r="Z10" s="58">
+      <c r="Z10" s="57">
         <v>37093.47</v>
       </c>
-      <c r="AA10" s="58">
+      <c r="AA10" s="57">
         <v>0</v>
       </c>
       <c r="AB10" s="40">
@@ -1728,12 +1728,12 @@
         <v>11</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q11" s="52">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="51">
         <v>285502.65000000002</v>
       </c>
-      <c r="R11" s="48">
+      <c r="R11" s="47">
         <v>490000</v>
       </c>
       <c r="S11" s="14">
@@ -1758,12 +1758,12 @@
         <v>11</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q12" s="52">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="51">
         <v>268303</v>
       </c>
-      <c r="R12" s="48">
+      <c r="R12" s="47">
         <v>500000</v>
       </c>
       <c r="S12" s="14">
@@ -1788,12 +1788,12 @@
         <v>14</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q13" s="52">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="51">
         <v>41821.550000000003</v>
       </c>
-      <c r="R13" s="48">
+      <c r="R13" s="47">
         <v>510000</v>
       </c>
       <c r="S13" s="14">
@@ -1818,12 +1818,12 @@
         <v>11</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q14" s="52">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="51">
         <v>297395.43</v>
       </c>
-      <c r="R14" s="48">
+      <c r="R14" s="47">
         <v>520000</v>
       </c>
       <c r="S14" s="14">
@@ -1848,12 +1848,12 @@
         <v>12</v>
       </c>
       <c r="P15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q15" s="53">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="52">
         <v>212339.41</v>
       </c>
-      <c r="R15" s="48">
+      <c r="R15" s="47">
         <v>520000</v>
       </c>
       <c r="S15" s="14">
@@ -1878,12 +1878,12 @@
         <v>12</v>
       </c>
       <c r="P16" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q16" s="53">
+        <v>47</v>
+      </c>
+      <c r="Q16" s="52">
         <v>319085.51</v>
       </c>
-      <c r="R16" s="48">
+      <c r="R16" s="47">
         <v>520000</v>
       </c>
       <c r="S16" s="14">
@@ -1903,15 +1903,15 @@
         <v>9</v>
       </c>
       <c r="O17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P17" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q17" s="53">
+        <v>48</v>
+      </c>
+      <c r="Q17" s="52">
         <v>174027.93</v>
       </c>
-      <c r="R17" s="48">
+      <c r="R17" s="47">
         <v>520000</v>
       </c>
       <c r="S17" s="14">
@@ -1928,18 +1928,18 @@
     </row>
     <row r="18" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O18" t="s">
         <v>11</v>
       </c>
       <c r="P18" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q18" s="53">
+        <v>49</v>
+      </c>
+      <c r="Q18" s="52">
         <v>206304.04</v>
       </c>
-      <c r="R18" s="48">
+      <c r="R18" s="47">
         <v>520000</v>
       </c>
       <c r="S18" s="14">
@@ -1972,6 +1972,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2002,18 +2003,18 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="13">
         <v>409020.28</v>
@@ -2026,7 +2027,7 @@
         <v>8.0799935017994914E-2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="32">
         <f>+D2*$F$29</f>
@@ -2035,7 +2036,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="13">
         <v>93468.21</v>
@@ -2048,7 +2049,7 @@
         <v>1.7816637306671539E-2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="32">
         <f t="shared" ref="G3:G27" si="1">+D3*$F$29</f>
@@ -2057,7 +2058,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="13">
         <v>68443.94</v>
@@ -2070,7 +2071,7 @@
         <v>1.2270123185586058E-2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="32">
         <f t="shared" si="1"/>
@@ -2079,7 +2080,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="13">
         <v>274170.09000000003</v>
@@ -2092,7 +2093,7 @@
         <v>3.708022648711426E-2</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="32">
         <f t="shared" si="1"/>
@@ -2101,7 +2102,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="13">
         <v>213670.02</v>
@@ -2114,7 +2115,7 @@
         <v>3.8238348707341857E-2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="32">
         <f t="shared" si="1"/>
@@ -2123,7 +2124,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="13">
         <v>406950.16</v>
@@ -2136,7 +2137,7 @@
         <v>5.9547046049244837E-2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="32">
         <f t="shared" si="1"/>
@@ -2145,7 +2146,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="13">
         <v>427264.27</v>
@@ -2158,7 +2159,7 @@
         <v>7.1517626963166908E-2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="32">
         <f t="shared" si="1"/>
@@ -2167,7 +2168,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13">
         <v>126634.43</v>
@@ -2180,7 +2181,7 @@
         <v>2.3660030530567734E-2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="32">
         <f t="shared" si="1"/>
@@ -2189,7 +2190,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="13">
         <v>236410.11</v>
@@ -2202,7 +2203,7 @@
         <v>3.6584243400356736E-2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" si="1"/>
@@ -2211,7 +2212,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="13">
         <v>262741.15000000002</v>
@@ -2224,7 +2225,7 @@
         <v>4.5317880441351911E-2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="32">
         <f t="shared" si="1"/>
@@ -2233,7 +2234,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="13">
         <v>245752.23</v>
@@ -2246,7 +2247,7 @@
         <v>4.2587777848449276E-2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="32">
         <f t="shared" si="1"/>
@@ -2255,7 +2256,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="13">
         <v>61149.25</v>
@@ -2268,7 +2269,7 @@
         <v>6.6383414196787638E-3</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="32">
         <f t="shared" si="1"/>
@@ -2277,7 +2278,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="13">
         <v>313310.19</v>
@@ -2290,7 +2291,7 @@
         <v>4.7205623582288608E-2</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="32">
         <f t="shared" si="1"/>
@@ -2299,7 +2300,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="16">
         <v>167888.82</v>
@@ -2312,7 +2313,7 @@
         <v>3.3704667672509861E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" s="32">
         <f t="shared" si="1"/>
@@ -2321,7 +2322,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="16">
         <v>279747.43</v>
@@ -2334,7 +2335,7 @@
         <v>5.0648492919253996E-2</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="32">
         <f t="shared" si="1"/>
@@ -2343,7 +2344,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="16">
         <v>166834.78</v>
@@ -2356,7 +2357,7 @@
         <v>2.7623481728721231E-2</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="32">
         <f t="shared" si="1"/>
@@ -2365,7 +2366,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="16">
         <v>199650.55</v>
@@ -2378,7 +2379,7 @@
         <v>3.2746673600199658E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G18" s="32">
         <f t="shared" si="1"/>
@@ -2387,7 +2388,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="8">
         <v>278034.96999999997</v>
@@ -2400,7 +2401,7 @@
         <v>3.8784920013770104E-2</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="32">
         <f t="shared" si="1"/>
@@ -2409,7 +2410,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="8">
         <v>359768.99</v>
@@ -2422,7 +2423,7 @@
         <v>3.9938580783925176E-2</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="32">
         <f t="shared" si="1"/>
@@ -2431,7 +2432,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="8">
         <v>309362.19</v>
@@ -2444,7 +2445,7 @@
         <v>5.9047733573258529E-2</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G21" s="32">
         <f t="shared" si="1"/>
@@ -2453,7 +2454,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="8">
         <v>106150.22</v>
@@ -2466,7 +2467,7 @@
         <v>2.1172168406439807E-2</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="32">
         <f t="shared" si="1"/>
@@ -2475,7 +2476,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="8">
         <v>253882.6</v>
@@ -2488,7 +2489,7 @@
         <v>4.533443832975928E-2</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" s="32">
         <f t="shared" si="1"/>
@@ -2497,7 +2498,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="8">
         <v>235058.47</v>
@@ -2510,7 +2511,7 @@
         <v>4.0428542197571374E-2</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="32">
         <f t="shared" si="1"/>
@@ -2519,7 +2520,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="8">
         <v>263862.83</v>
@@ -2532,7 +2533,7 @@
         <v>4.2009950701781637E-2</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G25" s="32">
         <f t="shared" si="1"/>
@@ -2541,7 +2542,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="8">
         <v>209021.72</v>
@@ -2554,7 +2555,7 @@
         <v>4.2943700517958767E-2</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" s="32">
         <f t="shared" si="1"/>
@@ -2563,7 +2564,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="8">
         <v>51752.1</v>
@@ -2576,7 +2577,7 @@
         <v>6.3528086150371407E-3</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27" s="32">
         <f t="shared" si="1"/>
@@ -2585,7 +2586,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F28" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G28" s="17">
         <v>6300000</v>
@@ -2630,15 +2631,15 @@
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G1" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>58</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="35">
         <v>282981.19</v>
@@ -2655,7 +2656,7 @@
         <v>6.8170046380641003E-2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="17">
         <f>+E2*$F$31</f>
@@ -2664,7 +2665,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="35">
         <v>59582.74</v>
@@ -2681,7 +2682,7 @@
         <v>1.4640475380660389E-2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" s="17">
         <f t="shared" ref="H3:H28" si="2">+E3*$F$31</f>
@@ -2690,7 +2691,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="35">
         <v>40250.339999999997</v>
@@ -2707,7 +2708,7 @@
         <v>1.1407324119862458E-2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="17">
         <f t="shared" si="2"/>
@@ -2716,7 +2717,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="36">
         <v>202775.76</v>
@@ -2733,7 +2734,7 @@
         <v>4.4445014401191481E-2</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="17">
         <f t="shared" si="2"/>
@@ -2742,7 +2743,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="35">
         <v>160934</v>
@@ -2759,7 +2760,7 @@
         <v>3.5611670556516144E-2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="17">
         <f t="shared" si="2"/>
@@ -2768,7 +2769,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="35">
         <v>297002.83</v>
@@ -2785,7 +2786,7 @@
         <v>6.7825026665540147E-2</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="17">
         <f t="shared" si="2"/>
@@ -2794,7 +2795,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="35">
         <v>283114.93</v>
@@ -2811,7 +2812,7 @@
         <v>7.1210711916227881E-2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" s="17">
         <f t="shared" si="2"/>
@@ -2820,7 +2821,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="35">
         <v>71683.649999999994</v>
@@ -2837,7 +2838,7 @@
         <v>1.9606006593439102E-2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" si="2"/>
@@ -2846,7 +2847,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="35">
         <v>161593.37</v>
@@ -2863,7 +2864,7 @@
         <v>3.9401684934949388E-2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" s="17">
         <f t="shared" si="2"/>
@@ -2872,7 +2873,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="35">
         <v>237983.01</v>
@@ -2889,7 +2890,7 @@
         <v>4.8790192137116405E-2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="17">
         <f t="shared" si="2"/>
@@ -2898,7 +2899,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="35">
         <f>81972.71+70013.19</f>
@@ -2916,7 +2917,7 @@
         <v>3.9708704374175181E-2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="17">
         <f t="shared" si="2"/>
@@ -2925,7 +2926,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="35">
         <v>42337.31</v>
@@ -2942,7 +2943,7 @@
         <v>9.706230707129981E-3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" si="2"/>
@@ -2951,7 +2952,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="35">
         <v>220828.11</v>
@@ -2968,7 +2969,7 @@
         <v>5.0968364201114447E-2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="17">
         <f t="shared" si="2"/>
@@ -2977,7 +2978,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="23">
         <v>126533.39</v>
@@ -2994,7 +2995,7 @@
         <v>2.7981470440763535E-2</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="17">
         <f t="shared" si="2"/>
@@ -3003,7 +3004,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="23">
         <v>174336.17</v>
@@ -3020,7 +3021,7 @@
         <v>4.6624572391056322E-2</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="17">
         <f t="shared" si="2"/>
@@ -3029,7 +3030,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="23">
         <v>113157.25</v>
@@ -3046,7 +3047,7 @@
         <v>2.78057959120659E-2</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H17" s="17">
         <f t="shared" si="2"/>
@@ -3055,7 +3056,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="23">
         <v>137376.89000000001</v>
@@ -3072,7 +3073,7 @@
         <v>3.2025091349522757E-2</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H18" s="17">
         <f t="shared" si="2"/>
@@ -3081,7 +3082,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="37">
         <v>254077.24</v>
@@ -3098,7 +3099,7 @@
         <v>4.633916117898472E-2</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" si="2"/>
@@ -3107,7 +3108,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="35">
         <v>357712.18</v>
@@ -3124,7 +3125,7 @@
         <v>5.9961498136912275E-2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" s="17">
         <f t="shared" si="2"/>
@@ -3133,7 +3134,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="35">
         <v>235041.5</v>
@@ -3150,7 +3151,7 @@
         <v>5.1560365173267723E-2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H21" s="17">
         <f t="shared" si="2"/>
@@ -3159,7 +3160,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="35">
         <v>89319.93</v>
@@ -3176,7 +3177,7 @@
         <v>1.7691702808738212E-2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="17">
         <f t="shared" si="2"/>
@@ -3185,7 +3186,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="35">
         <v>197098.61</v>
@@ -3202,7 +3203,7 @@
         <v>4.2313766880390118E-2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H23" s="17">
         <f t="shared" si="2"/>
@@ -3211,7 +3212,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="35">
         <v>225750.62</v>
@@ -3228,7 +3229,7 @@
         <v>3.9176411952891094E-2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="17">
         <f t="shared" si="2"/>
@@ -3237,7 +3238,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="35">
         <v>193932.79</v>
@@ -3254,7 +3255,7 @@
         <v>4.3977139098064173E-2</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="17">
         <f t="shared" si="2"/>
@@ -3263,7 +3264,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="35">
         <v>134166.89000000001</v>
@@ -3280,7 +3281,7 @@
         <v>3.4836953794004602E-2</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="17">
         <f t="shared" si="2"/>
@@ -3289,7 +3290,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="38">
         <v>33263.919999999998</v>
@@ -3306,7 +3307,7 @@
         <v>8.2146185147744816E-3</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" s="17">
         <f t="shared" si="2"/>
@@ -3322,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H28" s="17">
         <f t="shared" si="2"/>
@@ -3374,15 +3375,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="13">
         <v>409020.28</v>
@@ -3390,7 +3391,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="13">
         <v>93468.21</v>
@@ -3399,7 +3400,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="13">
         <v>68443.94</v>
@@ -3407,7 +3408,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="13">
         <v>274170.09000000003</v>
@@ -3415,7 +3416,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="13">
         <v>213670.02</v>
@@ -3423,7 +3424,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="13">
         <v>406950.16</v>
@@ -3431,7 +3432,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="13">
         <v>427264.27</v>
@@ -3439,7 +3440,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13">
         <v>126634.43</v>
@@ -3447,7 +3448,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="13">
         <v>236410.11</v>
@@ -3455,7 +3456,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="13">
         <v>262741.15000000002</v>
@@ -3463,7 +3464,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="13">
         <v>245752.23</v>
@@ -3471,7 +3472,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="13">
         <v>61149.25</v>
@@ -3480,7 +3481,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="13">
         <v>313310.19</v>
@@ -3488,7 +3489,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="16">
         <v>167888.82</v>
@@ -3496,7 +3497,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="16">
         <v>279747.43</v>
@@ -3504,7 +3505,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="16">
         <v>166834.78</v>
@@ -3512,7 +3513,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="16">
         <v>199650.55</v>
@@ -3520,7 +3521,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="8">
         <v>278034.96999999997</v>
@@ -3528,7 +3529,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="8">
         <v>359768.99</v>
@@ -3536,7 +3537,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="8">
         <v>309362.19</v>
@@ -3544,7 +3545,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="8">
         <v>106150.22</v>
@@ -3552,7 +3553,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="8">
         <v>253882.6</v>
@@ -3560,7 +3561,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="8">
         <v>235058.47</v>
@@ -3568,7 +3569,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="8">
         <v>263862.83</v>
@@ -3576,7 +3577,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="8">
         <v>209021.72</v>
@@ -3584,7 +3585,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="8">
         <v>51752.1</v>

</xml_diff>